<commit_message>
✨ feat(Helper.GlobalConfig): PLC connect
</commit_message>
<xml_diff>
--- a/com.myxmu.SCADASystem/Configs/TulingRead.xlsx
+++ b/com.myxmu.SCADASystem/Configs/TulingRead.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21942" windowHeight="10045"/>
+    <workbookView windowWidth="24685" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Read" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="202">
   <si>
     <t>Module</t>
   </si>
@@ -627,13 +627,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0."/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0."/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,9 +661,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -684,18 +690,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -708,6 +723,53 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -728,75 +790,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -813,13 +806,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,25 +848,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,7 +878,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,85 +962,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -969,31 +974,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,11 +1017,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1053,6 +1044,41 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1086,184 +1112,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1275,7 +1268,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1663,8 +1656,8 @@
   <sheetPr/>
   <dimension ref="A1:AA222"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
@@ -1756,7 +1749,9 @@
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1793,7 +1788,9 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1830,7 +1827,9 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1867,7 +1866,9 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1904,7 +1905,9 @@
       <c r="AA6" s="2"/>
     </row>
     <row r="7" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1941,7 +1944,9 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
@@ -1978,7 +1983,9 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
@@ -2015,7 +2022,9 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -2052,7 +2061,9 @@
       <c r="AA10" s="2"/>
     </row>
     <row r="11" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
@@ -2089,7 +2100,9 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
@@ -2126,7 +2139,9 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>40</v>
       </c>
@@ -2163,7 +2178,9 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B14" s="3" t="s">
         <v>43</v>
       </c>
@@ -2200,7 +2217,9 @@
       <c r="AA14" s="2"/>
     </row>
     <row r="15" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
@@ -2237,7 +2256,9 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>49</v>
       </c>
@@ -2274,7 +2295,9 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
@@ -2311,7 +2334,9 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
@@ -2348,7 +2373,9 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B19" s="3" t="s">
         <v>58</v>
       </c>
@@ -2385,7 +2412,9 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B20" s="3" t="s">
         <v>61</v>
       </c>
@@ -2422,7 +2451,9 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
@@ -2459,7 +2490,9 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B22" s="3" t="s">
         <v>67</v>
       </c>
@@ -2535,7 +2568,9 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>74</v>
       </c>
@@ -2572,7 +2607,9 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>77</v>
       </c>
@@ -2609,7 +2646,9 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>80</v>
       </c>
@@ -2646,7 +2685,9 @@
       <c r="AA26" s="2"/>
     </row>
     <row r="27" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>83</v>
       </c>
@@ -2683,7 +2724,9 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>86</v>
       </c>
@@ -2720,7 +2763,9 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>89</v>
       </c>
@@ -2757,7 +2802,9 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>92</v>
       </c>
@@ -2794,7 +2841,9 @@
       <c r="AA30" s="2"/>
     </row>
     <row r="31" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>95</v>
       </c>
@@ -2831,7 +2880,9 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>98</v>
       </c>
@@ -2868,7 +2919,9 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>101</v>
       </c>
@@ -2905,7 +2958,9 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>104</v>
       </c>
@@ -2942,7 +2997,9 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>107</v>
       </c>
@@ -2979,7 +3036,9 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>110</v>
       </c>
@@ -3016,7 +3075,9 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B37" s="2" t="s">
         <v>113</v>
       </c>
@@ -3053,7 +3114,9 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>116</v>
       </c>
@@ -3090,7 +3153,9 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
@@ -3127,7 +3192,9 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>122</v>
       </c>
@@ -3164,7 +3231,9 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B41" s="2" t="s">
         <v>125</v>
       </c>
@@ -3201,7 +3270,9 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>128</v>
       </c>
@@ -3238,7 +3309,9 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>131</v>
       </c>
@@ -3275,7 +3348,9 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>134</v>
       </c>
@@ -3312,7 +3387,9 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>137</v>
       </c>
@@ -3349,7 +3426,9 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>140</v>
       </c>
@@ -3386,7 +3465,9 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B47" s="2" t="s">
         <v>143</v>
       </c>
@@ -3423,7 +3504,9 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B48" s="2" t="s">
         <v>146</v>
       </c>
@@ -3460,7 +3543,9 @@
       <c r="AA48" s="2"/>
     </row>
     <row r="49" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B49" s="2" t="s">
         <v>149</v>
       </c>
@@ -3497,7 +3582,9 @@
       <c r="AA49" s="2"/>
     </row>
     <row r="50" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B50" s="2" t="s">
         <v>152</v>
       </c>
@@ -3534,7 +3621,9 @@
       <c r="AA50" s="2"/>
     </row>
     <row r="51" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="B51" s="2" t="s">
         <v>155</v>
       </c>
@@ -3610,7 +3699,9 @@
       <c r="AA52" s="2"/>
     </row>
     <row r="53" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B53" s="2" t="s">
         <v>163</v>
       </c>
@@ -3647,7 +3738,9 @@
       <c r="AA53" s="2"/>
     </row>
     <row r="54" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B54" s="2" t="s">
         <v>166</v>
       </c>
@@ -3684,7 +3777,9 @@
       <c r="AA54" s="2"/>
     </row>
     <row r="55" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B55" s="2" t="s">
         <v>169</v>
       </c>
@@ -3721,7 +3816,9 @@
       <c r="AA55" s="2"/>
     </row>
     <row r="56" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B56" s="2" t="s">
         <v>172</v>
       </c>
@@ -3758,7 +3855,9 @@
       <c r="AA56" s="2"/>
     </row>
     <row r="57" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B57" s="2" t="s">
         <v>175</v>
       </c>
@@ -3795,7 +3894,9 @@
       <c r="AA57" s="2"/>
     </row>
     <row r="58" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B58" s="2" t="s">
         <v>178</v>
       </c>
@@ -3832,7 +3933,9 @@
       <c r="AA58" s="2"/>
     </row>
     <row r="59" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B59" s="2" t="s">
         <v>181</v>
       </c>
@@ -3869,7 +3972,9 @@
       <c r="AA59" s="2"/>
     </row>
     <row r="60" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B60" s="3" t="s">
         <v>184</v>
       </c>
@@ -3906,7 +4011,9 @@
       <c r="AA60" s="2"/>
     </row>
     <row r="61" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B61" s="3" t="s">
         <v>187</v>
       </c>
@@ -3943,7 +4050,9 @@
       <c r="AA61" s="2"/>
     </row>
     <row r="62" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B62" s="3" t="s">
         <v>190</v>
       </c>
@@ -3980,7 +4089,9 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="63" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B63" s="3" t="s">
         <v>193</v>
       </c>
@@ -4017,7 +4128,9 @@
       <c r="AA63" s="2"/>
     </row>
     <row r="64" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B64" s="3" t="s">
         <v>196</v>
       </c>
@@ -4054,7 +4167,9 @@
       <c r="AA64" s="2"/>
     </row>
     <row r="65" ht="21.05" customHeight="1" spans="1:27">
-      <c r="A65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B65" s="3" t="s">
         <v>199</v>
       </c>
@@ -8588,10 +8703,7 @@
       <c r="AA222" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A22"/>
-    <mergeCell ref="A23:A51"/>
-    <mergeCell ref="A52:A65"/>
+  <mergeCells count="1">
     <mergeCell ref="A66:A79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>